<commit_message>
changed ADW sheet and added /ae
</commit_message>
<xml_diff>
--- a/data/excel files/in/statusReference.xlsx
+++ b/data/excel files/in/statusReference.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
   <si>
     <t>-</t>
   </si>
@@ -139,67 +139,70 @@
     <t>U/S</t>
   </si>
   <si>
+    <t>SITE ESCORT</t>
+  </si>
+  <si>
+    <t>RSAF55</t>
+  </si>
+  <si>
+    <t>DSO TRAINING</t>
+  </si>
+  <si>
+    <t>NDP</t>
+  </si>
+  <si>
+    <t>IMT</t>
+  </si>
+  <si>
+    <t>ATP IMT</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>O/S ME</t>
+  </si>
+  <si>
+    <t>202 SQN AUDIT</t>
+  </si>
+  <si>
+    <t>SITE FAM</t>
+  </si>
+  <si>
+    <t>CONVOY</t>
+  </si>
+  <si>
+    <t>CS IMT</t>
+  </si>
+  <si>
+    <t>GTT</t>
+  </si>
+  <si>
+    <t>SIC</t>
+  </si>
+  <si>
+    <t>RIGGER</t>
+  </si>
+  <si>
+    <t>GWT</t>
+  </si>
+  <si>
+    <t>OEMP</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>RDPC</t>
+  </si>
+  <si>
     <t>ESCORT</t>
-  </si>
-  <si>
-    <t>RSAF55</t>
-  </si>
-  <si>
-    <t>DSO TRAINING</t>
-  </si>
-  <si>
-    <t>NDP</t>
-  </si>
-  <si>
-    <t>IMT</t>
-  </si>
-  <si>
-    <t>ATP IMT</t>
-  </si>
-  <si>
-    <t>ATP</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>O/S ME</t>
-  </si>
-  <si>
-    <t>202 SQN AUDIT</t>
-  </si>
-  <si>
-    <t>SITE FAM</t>
-  </si>
-  <si>
-    <t>CONVOY</t>
-  </si>
-  <si>
-    <t>CS IMT</t>
-  </si>
-  <si>
-    <t>GTT</t>
-  </si>
-  <si>
-    <t>SIC</t>
-  </si>
-  <si>
-    <t>RIGGER</t>
-  </si>
-  <si>
-    <t>GWT</t>
-  </si>
-  <si>
-    <t>OEMP</t>
-  </si>
-  <si>
-    <t>CMD</t>
-  </si>
-  <si>
-    <t>RDPC</t>
   </si>
   <si>
     <t>CPC</t>
@@ -1001,7 +1004,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1393,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1401,16 +1404,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>